<commit_message>
AFDP-825 - DOL - OIG - Demo Tasks - update access control rules to deny access to non-participants when restricted flag is set on case files or complaints
</commit_message>
<xml_diff>
--- a/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-access-control-rules.xlsx
+++ b/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-access-control-rules.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="57">
   <si>
     <t>RuleSet</t>
   </si>
@@ -174,6 +174,15 @@
   </si>
   <si>
     <t>Case File – Lockout No Access Users</t>
+  </si>
+  <si>
+    <t>Complaint – Restricted Flag</t>
+  </si>
+  <si>
+    <t>restricted</t>
+  </si>
+  <si>
+    <t>Case File – Restricted Flag</t>
   </si>
   <si>
     <t>Object Types</t>
@@ -553,8 +562,8 @@
   </sheetPr>
   <dimension ref="A2:G32"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A13" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="D29" activeCellId="0" pane="topLeft" sqref="D29"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A7" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
+      <selection activeCell="B30" activeCellId="0" pane="topLeft" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3"/>
@@ -902,21 +911,37 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="28">
       <c r="A28" s="1"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
+      <c r="B28" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>47</v>
+      </c>
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="G28" s="18" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="29">
       <c r="A29" s="1"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
+      <c r="B29" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>47</v>
+      </c>
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="G29" s="18" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="30">
       <c r="A30" s="1"/>
@@ -976,10 +1001,10 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="2">
@@ -987,30 +1012,30 @@
         <v>31</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AFDP-835 - ARK-I - Close complaint/rework/resubmit tasks not showing on the task node in complaints module - grant read access by default to tasks
</commit_message>
<xml_diff>
--- a/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-access-control-rules.xlsx
+++ b/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-access-control-rules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="535" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="307" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="58">
   <si>
     <t>RuleSet</t>
   </si>
@@ -137,39 +137,39 @@
     <t>grant read to assignee</t>
   </si>
   <si>
-    <t>Complaint – Restrict Access to Drafts</t>
+    <t>Complaint – Grant Access to Drafts</t>
   </si>
   <si>
     <t>status == 'DRAFT'</t>
   </si>
   <si>
+    <t>grant read to *</t>
+  </si>
+  <si>
+    <t>Complaint – Grant Access to non-Drafts</t>
+  </si>
+  <si>
+    <t>status != 'DRAFT'</t>
+  </si>
+  <si>
+    <t>Complaint – Lockout No Access Users</t>
+  </si>
+  <si>
+    <t>mandatory deny read to No Access</t>
+  </si>
+  <si>
+    <t>Case File – Assignee Read Access</t>
+  </si>
+  <si>
+    <t>CASE_FILE</t>
+  </si>
+  <si>
+    <t>Case File – Restrict Access to Drafts</t>
+  </si>
+  <si>
     <t>deny read to *</t>
   </si>
   <si>
-    <t>Complaint – Grant Access to non-Drafts</t>
-  </si>
-  <si>
-    <t>status != 'DRAFT'</t>
-  </si>
-  <si>
-    <t>grant read to *</t>
-  </si>
-  <si>
-    <t>Complaint – Lockout No Access Users</t>
-  </si>
-  <si>
-    <t>mandatory deny read to No Access</t>
-  </si>
-  <si>
-    <t>Case File – Assignee Read Access</t>
-  </si>
-  <si>
-    <t>CASE_FILE</t>
-  </si>
-  <si>
-    <t>Case File – Restrict Access to Drafts</t>
-  </si>
-  <si>
     <t>Case File – Grant Access to non-Drafts</t>
   </si>
   <si>
@@ -185,6 +185,12 @@
     <t>Case File – Restricted Flag</t>
   </si>
   <si>
+    <t>Task – default read access</t>
+  </si>
+  <si>
+    <t>TASK</t>
+  </si>
+  <si>
     <t>Object Types</t>
   </si>
   <si>
@@ -192,9 +198,6 @@
   </si>
   <si>
     <t>Owner</t>
-  </si>
-  <si>
-    <t>TASK</t>
   </si>
   <si>
     <t>Owner's Supervisor</t>
@@ -562,8 +565,8 @@
   </sheetPr>
   <dimension ref="A2:G32"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A7" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="B30" activeCellId="0" pane="topLeft" sqref="B30"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A16" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
+      <selection activeCell="B31" activeCellId="0" pane="topLeft" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3"/>
@@ -796,7 +799,7 @@
         <v>32</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="24" outlineLevel="0" r="21">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.5" outlineLevel="0" r="21">
       <c r="A21" s="1"/>
       <c r="B21" s="16" t="s">
         <v>33</v>
@@ -827,13 +830,13 @@
       <c r="E22" s="18"/>
       <c r="F22" s="18"/>
       <c r="G22" s="18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.5" outlineLevel="0" r="23">
       <c r="A23" s="1"/>
       <c r="B23" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C23" s="18" t="s">
         <v>31</v>
@@ -842,16 +845,16 @@
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
       <c r="G23" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.65" outlineLevel="0" r="24">
       <c r="A24" s="1"/>
       <c r="B24" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="17" t="s">
         <v>41</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>42</v>
       </c>
       <c r="D24" s="17"/>
       <c r="E24" s="18"/>
@@ -863,10 +866,10 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.65" outlineLevel="0" r="25">
       <c r="A25" s="1"/>
       <c r="B25" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D25" s="17" t="s">
         <v>34</v>
@@ -874,7 +877,7 @@
       <c r="E25" s="18"/>
       <c r="F25" s="18"/>
       <c r="G25" s="18" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.65" outlineLevel="0" r="26">
@@ -883,7 +886,7 @@
         <v>44</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D26" s="17" t="s">
         <v>37</v>
@@ -891,7 +894,7 @@
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
       <c r="G26" s="18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.5" outlineLevel="0" r="27">
@@ -900,13 +903,13 @@
         <v>45</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D27" s="18"/>
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
       <c r="G27" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="28">
@@ -923,7 +926,7 @@
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
       <c r="G28" s="18" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="29">
@@ -932,7 +935,7 @@
         <v>48</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D29" s="18" t="s">
         <v>47</v>
@@ -940,17 +943,23 @@
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
       <c r="G29" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="30">
+        <v>43</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="30">
       <c r="A30" s="1"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="18"/>
+      <c r="B30" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>50</v>
+      </c>
       <c r="D30" s="18"/>
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="G30" s="18" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="31">
       <c r="A31" s="1"/>
@@ -1001,10 +1010,10 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="2">
@@ -1012,30 +1021,30 @@
         <v>31</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AFDP-162 - ACM permission evaluator - Allow granting a role to multiple permission types at once
</commit_message>
<xml_diff>
--- a/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-access-control-rules.xlsx
+++ b/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-access-control-rules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="307" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="169" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="70">
   <si>
     <t>RuleSet</t>
   </si>
@@ -158,6 +158,18 @@
     <t>mandatory deny read to No Access</t>
   </si>
   <si>
+    <t>Complaint – Only participants can add files</t>
+  </si>
+  <si>
+    <t>grant add file to assignee, co-owner, supervisor, owning group, approver, collaborator</t>
+  </si>
+  <si>
+    <t>Complaint – Only participants can save</t>
+  </si>
+  <si>
+    <t>grant save to assignee, co-owner, supervisor, owning group, approver, collaborator</t>
+  </si>
+  <si>
     <t>Case File – Assignee Read Access</t>
   </si>
   <si>
@@ -176,6 +188,12 @@
     <t>Case File – Lockout No Access Users</t>
   </si>
   <si>
+    <t>Case File – Only participants can add files</t>
+  </si>
+  <si>
+    <t>Case File – Only participants can save</t>
+  </si>
+  <si>
     <t>Complaint – Restricted Flag</t>
   </si>
   <si>
@@ -189,6 +207,24 @@
   </si>
   <si>
     <t>TASK</t>
+  </si>
+  <si>
+    <t>Task – Only participants can add files</t>
+  </si>
+  <si>
+    <t>Task – Only participants can save</t>
+  </si>
+  <si>
+    <t>Task – Only assignee can complete</t>
+  </si>
+  <si>
+    <t>grant complete to assignee</t>
+  </si>
+  <si>
+    <t>Task – Only assignee and supervisor can save</t>
+  </si>
+  <si>
+    <t>grant delete to assignee, supervisor</t>
   </si>
   <si>
     <t>Object Types</t>
@@ -563,13 +599,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:G32"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A16" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="B31" activeCellId="0" pane="topLeft" sqref="B31"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A13" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
+      <selection activeCell="H37" activeCellId="0" pane="topLeft" sqref="H37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.3"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.515306122449"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.2908163265306"/>
@@ -581,6 +617,7 @@
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="1"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
@@ -701,6 +738,7 @@
         <v>15</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="14"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="15">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
@@ -848,35 +886,33 @@
         <v>39</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.65" outlineLevel="0" r="24">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.65" outlineLevel="0" r="24">
       <c r="A24" s="1"/>
       <c r="B24" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="17" t="s">
-        <v>41</v>
+      <c r="C24" s="18" t="s">
+        <v>31</v>
       </c>
       <c r="D24" s="17"/>
       <c r="E24" s="18"/>
       <c r="F24" s="18"/>
-      <c r="G24" s="18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.65" outlineLevel="0" r="25">
+      <c r="G24" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="24" outlineLevel="0" r="25">
       <c r="A25" s="1"/>
       <c r="B25" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>34</v>
-      </c>
+      <c r="C25" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="17"/>
       <c r="E25" s="18"/>
       <c r="F25" s="18"/>
-      <c r="G25" s="18" t="s">
+      <c r="G25" s="16" t="s">
         <v>43</v>
       </c>
     </row>
@@ -886,98 +922,211 @@
         <v>44</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>37</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="D26" s="17"/>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
       <c r="G26" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.5" outlineLevel="0" r="27">
+        <v>32</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.65" outlineLevel="0" r="27">
       <c r="A27" s="1"/>
       <c r="B27" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" s="18"/>
+      <c r="D27" s="17" t="s">
+        <v>34</v>
+      </c>
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
       <c r="G27" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="28">
+        <v>47</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.65" outlineLevel="0" r="28">
       <c r="A28" s="1"/>
       <c r="B28" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" s="18" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>37</v>
       </c>
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
       <c r="G28" s="18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="29">
+        <v>35</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.5" outlineLevel="0" r="29">
       <c r="A29" s="1"/>
       <c r="B29" s="16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D29" s="18" t="s">
-        <v>47</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="D29" s="18"/>
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
       <c r="G29" s="18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="30">
+        <v>39</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="30">
       <c r="A30" s="1"/>
       <c r="B30" s="16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" s="18"/>
+        <v>45</v>
+      </c>
+      <c r="D30" s="17"/>
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
-      <c r="G30" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="31">
+      <c r="G30" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="31">
       <c r="A31" s="1"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
+      <c r="B31" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="17"/>
       <c r="E31" s="18"/>
       <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="G31" s="16" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="32">
       <c r="A32" s="1"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="B32" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>53</v>
+      </c>
       <c r="E32" s="18"/>
       <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="G32" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="33">
+      <c r="A33" s="1"/>
+      <c r="B33" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="34">
+      <c r="A34" s="1"/>
+      <c r="B34" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="35">
+      <c r="A35" s="1"/>
+      <c r="B35" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" s="17"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="36">
+      <c r="A36" s="1"/>
+      <c r="B36" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D36" s="17"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="24" outlineLevel="0" r="37">
+      <c r="A37" s="1"/>
+      <c r="B37" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" s="17"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="24" outlineLevel="0" r="38">
+      <c r="A38" s="1"/>
+      <c r="B38" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D38" s="17"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="39">
+      <c r="A39" s="1"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1010,10 +1159,10 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="2">
@@ -1021,30 +1170,30 @@
         <v>31</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AFDP-927 - Case file restricted flag not working as expected - update access rules to let participants view draft case files
</commit_message>
<xml_diff>
--- a/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-access-control-rules.xlsx
+++ b/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-access-control-rules.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="71">
   <si>
     <t>RuleSet</t>
   </si>
@@ -176,28 +176,31 @@
     <t>CASE_FILE</t>
   </si>
   <si>
-    <t>Case File – Restrict Access to Drafts</t>
+    <t>Case File – Grant Participants Access to Drafts</t>
+  </si>
+  <si>
+    <t>grant read to assignee, co-owner, supervisor, owning group, approver, collaborator, follower, reader</t>
+  </si>
+  <si>
+    <t>Case File – Grant Access to non-Drafts</t>
+  </si>
+  <si>
+    <t>Case File – Lockout No Access Users</t>
+  </si>
+  <si>
+    <t>Case File – Only participants can add files</t>
+  </si>
+  <si>
+    <t>Case File – Only participants can save</t>
+  </si>
+  <si>
+    <t>Complaint – Restricted Flag</t>
+  </si>
+  <si>
+    <t>restricted</t>
   </si>
   <si>
     <t>deny read to *</t>
-  </si>
-  <si>
-    <t>Case File – Grant Access to non-Drafts</t>
-  </si>
-  <si>
-    <t>Case File – Lockout No Access Users</t>
-  </si>
-  <si>
-    <t>Case File – Only participants can add files</t>
-  </si>
-  <si>
-    <t>Case File – Only participants can save</t>
-  </si>
-  <si>
-    <t>Complaint – Restricted Flag</t>
-  </si>
-  <si>
-    <t>restricted</t>
   </si>
   <si>
     <t>Case File – Restricted Flag</t>
@@ -602,7 +605,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A13" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="H37" activeCellId="0" pane="topLeft" sqref="H37"/>
+      <selection activeCell="G28" activeCellId="0" pane="topLeft" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -931,7 +934,7 @@
         <v>32</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.65" outlineLevel="0" r="27">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.65" outlineLevel="0" r="27">
       <c r="A27" s="1"/>
       <c r="B27" s="16" t="s">
         <v>46</v>
@@ -944,7 +947,7 @@
       </c>
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
-      <c r="G27" s="18" t="s">
+      <c r="G27" s="16" t="s">
         <v>47</v>
       </c>
     </row>
@@ -995,7 +998,7 @@
         <v>41</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="31">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="24" outlineLevel="0" r="31">
       <c r="A31" s="1"/>
       <c r="B31" s="16" t="s">
         <v>51</v>
@@ -1024,13 +1027,13 @@
       <c r="E32" s="18"/>
       <c r="F32" s="18"/>
       <c r="G32" s="18" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="33">
       <c r="A33" s="1"/>
       <c r="B33" s="16" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C33" s="18" t="s">
         <v>45</v>
@@ -1041,16 +1044,16 @@
       <c r="E33" s="18"/>
       <c r="F33" s="18"/>
       <c r="G33" s="18" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="34">
       <c r="A34" s="1"/>
       <c r="B34" s="16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D34" s="18"/>
       <c r="E34" s="18"/>
@@ -1062,10 +1065,10 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="35">
       <c r="A35" s="1"/>
       <c r="B35" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" s="18" t="s">
         <v>57</v>
-      </c>
-      <c r="C35" s="18" t="s">
-        <v>56</v>
       </c>
       <c r="D35" s="17"/>
       <c r="E35" s="18"/>
@@ -1077,10 +1080,10 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="36">
       <c r="A36" s="1"/>
       <c r="B36" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D36" s="17"/>
       <c r="E36" s="18"/>
@@ -1092,31 +1095,31 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="24" outlineLevel="0" r="37">
       <c r="A37" s="1"/>
       <c r="B37" s="16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D37" s="17"/>
       <c r="E37" s="18"/>
       <c r="F37" s="18"/>
       <c r="G37" s="16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="24" outlineLevel="0" r="38">
       <c r="A38" s="1"/>
       <c r="B38" s="16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D38" s="17"/>
       <c r="E38" s="18"/>
       <c r="F38" s="18"/>
       <c r="G38" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="39">
@@ -1159,10 +1162,10 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="2">
@@ -1170,30 +1173,30 @@
         <v>31</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AFDP-1050 - Implement Document level security - initial implementation of folder security
</commit_message>
<xml_diff>
--- a/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-access-control-rules.xlsx
+++ b/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-access-control-rules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="169" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="169" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="73">
   <si>
     <t>RuleSet</t>
   </si>
@@ -230,6 +230,12 @@
     <t>grant delete to assignee, supervisor</t>
   </si>
   <si>
+    <t>Folder – default public access</t>
+  </si>
+  <si>
+    <t>FOLDER</t>
+  </si>
+  <si>
     <t>Object Types</t>
   </si>
   <si>
@@ -256,8 +262,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;" numFmtId="165"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -341,77 +347,77 @@
     </fill>
   </fills>
   <borders count="11">
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left style="medium"/>
       <right style="thin"/>
       <top style="medium"/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right style="medium"/>
       <top style="medium"/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left style="medium"/>
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right style="medium"/>
       <top style="thin"/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left style="medium"/>
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="medium"/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right style="medium"/>
       <top style="thin"/>
       <bottom style="medium"/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left style="medium"/>
       <right style="medium"/>
       <top style="thin"/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left style="medium"/>
       <right style="thin"/>
       <top style="thin"/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right style="thin"/>
       <top/>
@@ -420,119 +426,119 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="20">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="3" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="7" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="5" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="6" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="7" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="7" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="8" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="0" fontId="0" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -600,12 +606,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A13" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="G28" activeCellId="0" pane="topLeft" sqref="G28"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G40" activeCellId="0" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -620,8 +627,8 @@
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="1"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
+    <row r="1" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -631,7 +638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -641,7 +648,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
+    <row r="4" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -651,7 +658,7 @@
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5">
+    <row r="5" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -661,7 +668,7 @@
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
+    <row r="6" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -671,7 +678,7 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
+    <row r="7" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -681,7 +688,7 @@
         <v>7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="8">
+    <row r="8" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -691,7 +698,7 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
+    <row r="9" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -701,7 +708,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="10">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -711,7 +718,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11">
+    <row r="11" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
@@ -721,7 +728,7 @@
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="255.7" outlineLevel="0" r="12">
+    <row r="12" customFormat="false" ht="255.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="4" t="s">
@@ -731,7 +738,7 @@
         <v>13</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="13">
+    <row r="13" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="7" t="s">
@@ -741,8 +748,8 @@
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="14"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="15">
+    <row r="14" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
@@ -753,7 +760,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="16">
+    <row r="16" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="4" t="s">
@@ -772,7 +779,7 @@
         <v>18</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="17">
+    <row r="17" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="4" t="s">
@@ -783,7 +790,7 @@
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="18">
+    <row r="18" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="10" t="s">
@@ -802,7 +809,7 @@
         <v>22</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="68.65" outlineLevel="0" r="19">
+    <row r="19" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11" t="s">
         <v>23</v>
       </c>
@@ -825,7 +832,7 @@
         <v>29</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="24" outlineLevel="0" r="20">
+    <row r="20" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1"/>
       <c r="B20" s="16" t="s">
         <v>30</v>
@@ -840,7 +847,7 @@
         <v>32</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.5" outlineLevel="0" r="21">
+    <row r="21" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1"/>
       <c r="B21" s="16" t="s">
         <v>33</v>
@@ -857,7 +864,7 @@
         <v>35</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.5" outlineLevel="0" r="22">
+    <row r="22" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1"/>
       <c r="B22" s="16" t="s">
         <v>36</v>
@@ -874,7 +881,7 @@
         <v>35</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.5" outlineLevel="0" r="23">
+    <row r="23" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1"/>
       <c r="B23" s="16" t="s">
         <v>38</v>
@@ -889,7 +896,7 @@
         <v>39</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.65" outlineLevel="0" r="24">
+    <row r="24" customFormat="false" ht="35.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1"/>
       <c r="B24" s="16" t="s">
         <v>40</v>
@@ -904,7 +911,7 @@
         <v>41</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="24" outlineLevel="0" r="25">
+    <row r="25" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1"/>
       <c r="B25" s="16" t="s">
         <v>42</v>
@@ -919,7 +926,7 @@
         <v>43</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.65" outlineLevel="0" r="26">
+    <row r="26" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1"/>
       <c r="B26" s="16" t="s">
         <v>44</v>
@@ -934,7 +941,7 @@
         <v>32</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.65" outlineLevel="0" r="27">
+    <row r="27" customFormat="false" ht="35.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1"/>
       <c r="B27" s="16" t="s">
         <v>46</v>
@@ -951,7 +958,7 @@
         <v>47</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.65" outlineLevel="0" r="28">
+    <row r="28" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1"/>
       <c r="B28" s="16" t="s">
         <v>48</v>
@@ -968,7 +975,7 @@
         <v>35</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.5" outlineLevel="0" r="29">
+    <row r="29" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1"/>
       <c r="B29" s="16" t="s">
         <v>49</v>
@@ -983,7 +990,7 @@
         <v>39</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="30">
+    <row r="30" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1"/>
       <c r="B30" s="16" t="s">
         <v>50</v>
@@ -998,7 +1005,7 @@
         <v>41</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="24" outlineLevel="0" r="31">
+    <row r="31" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1"/>
       <c r="B31" s="16" t="s">
         <v>51</v>
@@ -1013,7 +1020,7 @@
         <v>43</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="32">
+    <row r="32" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1"/>
       <c r="B32" s="16" t="s">
         <v>52</v>
@@ -1030,7 +1037,7 @@
         <v>54</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="33">
+    <row r="33" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1"/>
       <c r="B33" s="16" t="s">
         <v>55</v>
@@ -1047,7 +1054,7 @@
         <v>54</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="34">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1"/>
       <c r="B34" s="16" t="s">
         <v>56</v>
@@ -1062,7 +1069,7 @@
         <v>35</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="35">
+    <row r="35" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1"/>
       <c r="B35" s="16" t="s">
         <v>58</v>
@@ -1077,7 +1084,7 @@
         <v>41</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="36">
+    <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1"/>
       <c r="B36" s="16" t="s">
         <v>59</v>
@@ -1092,7 +1099,7 @@
         <v>43</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="24" outlineLevel="0" r="37">
+    <row r="37" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1"/>
       <c r="B37" s="16" t="s">
         <v>60</v>
@@ -1107,7 +1114,7 @@
         <v>61</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="24" outlineLevel="0" r="38">
+    <row r="38" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1"/>
       <c r="B38" s="16" t="s">
         <v>62</v>
@@ -1122,19 +1129,25 @@
         <v>63</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="39">
+    <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="18"/>
+      <c r="B39" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>65</v>
+      </c>
       <c r="D39" s="18"/>
       <c r="E39" s="18"/>
       <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
+      <c r="G39" s="18" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1145,12 +1158,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1160,49 +1174,49 @@
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="4">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.55" outlineLevel="0" r="6">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1213,12 +1227,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1228,7 +1243,7 @@
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
AFDP-1050 - Implement Document level security - configuration file updates
</commit_message>
<xml_diff>
--- a/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-access-control-rules.xlsx
+++ b/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-access-control-rules.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="74">
   <si>
     <t>RuleSet</t>
   </si>
@@ -234,6 +234,9 @@
   </si>
   <si>
     <t>FOLDER</t>
+  </si>
+  <si>
+    <t>Folder –deny no access</t>
   </si>
   <si>
     <t>Object Types</t>
@@ -606,13 +609,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G40" activeCellId="0" sqref="G40"/>
+      <selection pane="topLeft" activeCell="B40" activeCellId="0" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1144,6 +1147,21 @@
         <v>35</v>
       </c>
     </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1"/>
+      <c r="B40" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1158,7 +1176,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B6"/>
@@ -1176,10 +1194,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1187,7 +1205,7 @@
         <v>31</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1195,22 +1213,22 @@
         <v>57</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1227,7 +1245,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>

</xml_diff>

<commit_message>
AFDP-1108 - Logical delete of case files - add DELETED status, make DELETED files inaccessible
</commit_message>
<xml_diff>
--- a/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-access-control-rules.xlsx
+++ b/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-access-control-rules.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="77">
   <si>
     <t>RuleSet</t>
   </si>
@@ -192,6 +192,15 @@
   </si>
   <si>
     <t>Case File – Only participants can save</t>
+  </si>
+  <si>
+    <t>Case File – Deleted Cases</t>
+  </si>
+  <si>
+    <t>status == 'DELETED'</t>
+  </si>
+  <si>
+    <t>mandatory deny read to assignee, co-owner, supervisor, owning group, approver, collaborator, *</t>
   </si>
   <si>
     <t>Complaint – Restricted Flag</t>
@@ -612,10 +621,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B40" activeCellId="0" sqref="B40"/>
+      <selection pane="topLeft" activeCell="G33" activeCellId="0" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1023,20 +1032,20 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1"/>
       <c r="B32" s="16" t="s">
         <v>52</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D32" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="17" t="s">
         <v>53</v>
       </c>
       <c r="E32" s="18"/>
       <c r="F32" s="18"/>
-      <c r="G32" s="18" t="s">
+      <c r="G32" s="16" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1046,119 +1055,136 @@
         <v>55</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E33" s="18"/>
       <c r="F33" s="18"/>
       <c r="G33" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1"/>
       <c r="B34" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="C34" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="D34" s="18"/>
       <c r="E34" s="18"/>
       <c r="F34" s="18"/>
       <c r="G34" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1"/>
       <c r="B35" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="D35" s="17"/>
+        <v>60</v>
+      </c>
+      <c r="D35" s="18"/>
       <c r="E35" s="18"/>
       <c r="F35" s="18"/>
-      <c r="G35" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G35" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1"/>
       <c r="B36" s="16" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D36" s="17"/>
       <c r="E36" s="18"/>
       <c r="F36" s="18"/>
       <c r="G36" s="16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1"/>
       <c r="B37" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" s="18" t="s">
         <v>60</v>
-      </c>
-      <c r="C37" s="18" t="s">
-        <v>57</v>
       </c>
       <c r="D37" s="17"/>
       <c r="E37" s="18"/>
       <c r="F37" s="18"/>
       <c r="G37" s="16" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1"/>
       <c r="B38" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D38" s="17"/>
       <c r="E38" s="18"/>
       <c r="F38" s="18"/>
       <c r="G38" s="16" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1"/>
       <c r="B39" s="16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="D39" s="18"/>
+        <v>60</v>
+      </c>
+      <c r="D39" s="17"/>
       <c r="E39" s="18"/>
       <c r="F39" s="18"/>
-      <c r="G39" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G39" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1"/>
       <c r="B40" s="16" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D40" s="18"/>
       <c r="E40" s="18"/>
       <c r="F40" s="18"/>
       <c r="G40" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1"/>
+      <c r="B41" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1194,10 +1220,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1205,30 +1231,30 @@
         <v>31</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SBI-975 - Update data access rules and assignment rules for Bactes - add DAC rules for the new permissions added to bactes
</commit_message>
<xml_diff>
--- a/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-access-control-rules.xlsx
+++ b/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-access-control-rules.xlsx
@@ -1,27 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DMILLE~1.ARM\ONEDRI~2\DOCUME~1\MobaXterm\slash\RemoteFiles\4\armdev@devvm\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="169" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="169"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="ObjectTypes" vbProcedure="false">Sheet2!$A$2:$A$51</definedName>
-    <definedName function="false" hidden="false" name="ParticipantTypes" vbProcedure="false">Sheet2!$B$2:$B$51</definedName>
+    <definedName name="ObjectTypes">Sheet2!$A$2:$A$51</definedName>
+    <definedName name="ParticipantTypes">Sheet2!$B$2:$B$51</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="95">
   <si>
     <t>RuleSet</t>
   </si>
@@ -233,9 +237,6 @@
     <t>grant complete to assignee</t>
   </si>
   <si>
-    <t>Task – Only assignee and supervisor can save</t>
-  </si>
-  <si>
     <t>grant delete to assignee, supervisor</t>
   </si>
   <si>
@@ -267,38 +268,79 @@
   </si>
   <si>
     <t>ACCESS CONTROL LIST</t>
+  </si>
+  <si>
+    <t>grant uploadOrReplaceFile to assignee, co-owner, supervisor, owning group, approver, collaborator</t>
+  </si>
+  <si>
+    <t>Complaint – Only participants can upload or replace files</t>
+  </si>
+  <si>
+    <t>Complaint – Anybody can add comments</t>
+  </si>
+  <si>
+    <t>Complaint – Anybody can subscribe</t>
+  </si>
+  <si>
+    <t>grant addComment to *</t>
+  </si>
+  <si>
+    <t>grant subscribe to *</t>
+  </si>
+  <si>
+    <t>grant viewCaseDetailsPage to assignee, co-owner, supervisor, owning group, approver, collaborator, reader</t>
+  </si>
+  <si>
+    <t>grant saveCase to assignee, co-owner, supervisor, owning group, approver, collaborator</t>
+  </si>
+  <si>
+    <t>Case File – Only participants can view details page</t>
+  </si>
+  <si>
+    <t>Case File – Only participants can version files</t>
+  </si>
+  <si>
+    <t>grant uploadOrReplaceFile to assignee, co-owner, supervisor, owning group, approver, collaborator, reader</t>
+  </si>
+  <si>
+    <t>grant addComment to assignee, co-owner, supervisor, owning group, approver, collaborator, reader</t>
+  </si>
+  <si>
+    <t>Case File – Only participants can add comments</t>
+  </si>
+  <si>
+    <t>Case File – anyone can subscribe</t>
+  </si>
+  <si>
+    <t>Task – Only assignee and supervisor can delete</t>
+  </si>
+  <si>
+    <t>grant subscribe to subscribe</t>
+  </si>
+  <si>
+    <t>Task – anybody can subscribe</t>
+  </si>
+  <si>
+    <t>Task – Only participants can add comments</t>
+  </si>
+  <si>
+    <t>Task – Only participants can version files</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -359,199 +401,202 @@
     </fill>
   </fills>
   <borders count="11">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -610,37 +655,312 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G41"/>
+  <dimension ref="A2:G52"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G33" activeCellId="0" sqref="G33"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.515306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.2908163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.9030612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.0765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.9183673469388"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.5102040816327"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.6020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="21.5703125"/>
+    <col min="2" max="2" width="24.28515625"/>
+    <col min="3" max="3" width="49.85546875"/>
+    <col min="4" max="4" width="36.140625"/>
+    <col min="5" max="5" width="43.85546875"/>
+    <col min="6" max="6" width="30.5703125"/>
+    <col min="7" max="7" width="35.5703125"/>
+    <col min="8" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="2" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -650,7 +970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -660,7 +980,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -670,7 +990,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -680,7 +1000,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -690,7 +1010,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -700,7 +1020,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -710,7 +1030,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -720,7 +1040,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -730,7 +1050,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
@@ -740,7 +1060,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="255.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:7" ht="360" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="4" t="s">
@@ -750,7 +1070,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="7" t="s">
@@ -760,8 +1080,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
@@ -772,7 +1091,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="4" t="s">
@@ -791,7 +1110,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="4" t="s">
@@ -802,7 +1121,7 @@
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="10" t="s">
@@ -821,7 +1140,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>23</v>
       </c>
@@ -844,7 +1163,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="16" t="s">
         <v>30</v>
@@ -859,7 +1178,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="16" t="s">
         <v>33</v>
@@ -876,7 +1195,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="16" t="s">
         <v>36</v>
@@ -893,7 +1212,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="16" t="s">
         <v>38</v>
@@ -908,7 +1227,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="35.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="16" t="s">
         <v>40</v>
@@ -923,7 +1242,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="16" t="s">
         <v>42</v>
@@ -938,359 +1257,505 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>45</v>
+        <v>77</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>31</v>
       </c>
       <c r="D26" s="17"/>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
-      <c r="G26" s="18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="35.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G26" s="16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>34</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="17"/>
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
       <c r="G27" s="16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>37</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="17"/>
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
-      <c r="G28" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G28" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D29" s="18"/>
+      <c r="D29" s="17"/>
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
       <c r="G29" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D30" s="17"/>
+      <c r="D30" s="17" t="s">
+        <v>34</v>
+      </c>
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
       <c r="G30" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C31" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D31" s="17"/>
+      <c r="D31" s="17" t="s">
+        <v>37</v>
+      </c>
       <c r="E31" s="18"/>
       <c r="F31" s="18"/>
-      <c r="G31" s="16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G31" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="16" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C32" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D32" s="17" t="s">
-        <v>53</v>
-      </c>
+      <c r="D32" s="18"/>
       <c r="E32" s="18"/>
       <c r="F32" s="18"/>
-      <c r="G32" s="16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G32" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="16" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D33" s="18" t="s">
-        <v>56</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="D33" s="17"/>
       <c r="E33" s="18"/>
       <c r="F33" s="18"/>
-      <c r="G33" s="18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G33" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="16" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C34" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D34" s="18" t="s">
-        <v>56</v>
-      </c>
+      <c r="D34" s="17"/>
       <c r="E34" s="18"/>
       <c r="F34" s="18"/>
-      <c r="G34" s="18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G34" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="16" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D35" s="18"/>
+        <v>45</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>53</v>
+      </c>
       <c r="E35" s="18"/>
       <c r="F35" s="18"/>
-      <c r="G35" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G35" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="16" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D36" s="17"/>
+        <v>31</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>56</v>
+      </c>
       <c r="E36" s="18"/>
       <c r="F36" s="18"/>
-      <c r="G36" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G36" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="16" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D37" s="17"/>
+        <v>45</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>56</v>
+      </c>
       <c r="E37" s="18"/>
       <c r="F37" s="18"/>
-      <c r="G37" s="16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G37" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="16" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="D38" s="17"/>
       <c r="E38" s="18"/>
       <c r="F38" s="18"/>
       <c r="G38" s="16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="16" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="D39" s="17"/>
       <c r="E39" s="18"/>
       <c r="F39" s="18"/>
       <c r="G39" s="16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="16" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="D40" s="18"/>
+        <v>45</v>
+      </c>
+      <c r="D40" s="17"/>
       <c r="E40" s="18"/>
       <c r="F40" s="18"/>
-      <c r="G40" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G40" s="16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="16" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="D41" s="18"/>
+        <v>45</v>
+      </c>
+      <c r="D41" s="17"/>
       <c r="E41" s="18"/>
       <c r="F41" s="18"/>
-      <c r="G41" s="18" t="s">
+      <c r="G41" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D42" s="17"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+      <c r="B44" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D44" s="17"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+      <c r="B45" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D45" s="17"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="B46" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D46" s="17"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D47" s="17"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+      <c r="B48" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D48" s="17"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+      <c r="B49" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D49" s="17"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
+      <c r="B50" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D50" s="17"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+      <c r="B51" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+      <c r="B52" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="18" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="18.7109375"/>
+    <col min="2" max="2" width="17.5703125"/>
+    <col min="3" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="0" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="0" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="0" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>76</v>
-      </c>
-    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified task, case and complaint rules when status is CLOSED. Added missing MessageService in complaint and task controllers. Updated participants and privileges when task is closed.
Former-commit-id: d1c4f5f807101c773d79b777313748bde1afa850
</commit_message>
<xml_diff>
--- a/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-access-control-rules.xlsx
+++ b/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-access-control-rules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DMILLE~1.ARM\ONEDRI~2\DOCUME~1\MobaXterm\slash\RemoteFiles\4\armdev@devvm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sasko.tanaskoski\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="102">
   <si>
     <t>RuleSet</t>
   </si>
@@ -325,6 +325,27 @@
   </si>
   <si>
     <t>Task – Only participants can version files</t>
+  </si>
+  <si>
+    <t>status != 'CLOSED'</t>
+  </si>
+  <si>
+    <t>status == 'CLOSED'</t>
+  </si>
+  <si>
+    <t>deny uploadOrReplaceFile to assignee, co-owner, supervisor, owning group, approver, collaborator</t>
+  </si>
+  <si>
+    <t>Case File – Participants cannot version files</t>
+  </si>
+  <si>
+    <t>Task – Participants cannot version files</t>
+  </si>
+  <si>
+    <t>Complaint – Participants cannot upload or replace files</t>
+  </si>
+  <si>
+    <t>deny uploadOrReplaceFile to assignee, co-owner, supervisor, owning group, approver, collaborator, reader</t>
   </si>
 </sst>
 </file>
@@ -752,6 +773,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -787,6 +825,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -942,10 +997,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A2:G52"/>
+  <dimension ref="A2:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1265,32 +1320,36 @@
       <c r="C26" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="17"/>
+      <c r="D26" s="17" t="s">
+        <v>95</v>
+      </c>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
       <c r="G26" s="16" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="16" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="C27" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="17"/>
+      <c r="D27" s="17" t="s">
+        <v>96</v>
+      </c>
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
       <c r="G27" s="16" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C28" s="18" t="s">
         <v>31</v>
@@ -1299,92 +1358,92 @@
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
       <c r="G28" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>45</v>
+        <v>79</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>31</v>
       </c>
       <c r="D29" s="17"/>
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
-      <c r="G29" s="18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G29" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C30" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D30" s="17" t="s">
-        <v>34</v>
-      </c>
+      <c r="D30" s="17"/>
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
-      <c r="G30" s="16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G30" s="18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C31" s="17" t="s">
         <v>45</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E31" s="18"/>
       <c r="F31" s="18"/>
-      <c r="G31" s="18" t="s">
-        <v>35</v>
+      <c r="G31" s="16" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D32" s="18"/>
+      <c r="D32" s="17" t="s">
+        <v>37</v>
+      </c>
       <c r="E32" s="18"/>
       <c r="F32" s="18"/>
       <c r="G32" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C33" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="17"/>
+      <c r="D33" s="18"/>
       <c r="E33" s="18"/>
       <c r="F33" s="18"/>
-      <c r="G33" s="16" t="s">
-        <v>41</v>
+      <c r="G33" s="18" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C34" s="18" t="s">
         <v>45</v>
@@ -1393,50 +1452,48 @@
       <c r="E34" s="18"/>
       <c r="F34" s="18"/>
       <c r="G34" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C35" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D35" s="17" t="s">
-        <v>53</v>
-      </c>
+      <c r="D35" s="17"/>
       <c r="E35" s="18"/>
       <c r="F35" s="18"/>
       <c r="G35" s="16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D36" s="18" t="s">
-        <v>56</v>
+        <v>45</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>53</v>
       </c>
       <c r="E36" s="18"/>
       <c r="F36" s="18"/>
-      <c r="G36" s="18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G36" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D37" s="18" t="s">
         <v>56</v>
@@ -1447,25 +1504,27 @@
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="16" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="C38" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D38" s="17"/>
+      <c r="D38" s="18" t="s">
+        <v>56</v>
+      </c>
       <c r="E38" s="18"/>
       <c r="F38" s="18"/>
-      <c r="G38" s="16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G38" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="16" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="C39" s="18" t="s">
         <v>45</v>
@@ -1474,13 +1533,13 @@
       <c r="E39" s="18"/>
       <c r="F39" s="18"/>
       <c r="G39" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="16" t="s">
-        <v>85</v>
+        <v>51</v>
       </c>
       <c r="C40" s="18" t="s">
         <v>45</v>
@@ -1489,88 +1548,92 @@
       <c r="E40" s="18"/>
       <c r="F40" s="18"/>
       <c r="G40" s="16" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="16" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C41" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D41" s="17"/>
+      <c r="D41" s="17" t="s">
+        <v>95</v>
+      </c>
       <c r="E41" s="18"/>
       <c r="F41" s="18"/>
       <c r="G41" s="16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="16" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="C42" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D42" s="17"/>
+      <c r="D42" s="17" t="s">
+        <v>96</v>
+      </c>
       <c r="E42" s="18"/>
       <c r="F42" s="18"/>
       <c r="G42" s="16" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="16" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D43" s="18"/>
+        <v>45</v>
+      </c>
+      <c r="D43" s="17"/>
       <c r="E43" s="18"/>
       <c r="F43" s="18"/>
-      <c r="G43" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G43" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="16" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="D44" s="17"/>
       <c r="E44" s="18"/>
       <c r="F44" s="18"/>
       <c r="G44" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C45" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D45" s="17"/>
+      <c r="D45" s="18"/>
       <c r="E45" s="18"/>
       <c r="F45" s="18"/>
-      <c r="G45" s="16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G45" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C46" s="18" t="s">
         <v>60</v>
@@ -1579,13 +1642,13 @@
       <c r="E46" s="18"/>
       <c r="F46" s="18"/>
       <c r="G46" s="16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="16" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="C47" s="18" t="s">
         <v>60</v>
@@ -1594,13 +1657,13 @@
       <c r="E47" s="18"/>
       <c r="F47" s="18"/>
       <c r="G47" s="16" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="16" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="C48" s="18" t="s">
         <v>60</v>
@@ -1609,13 +1672,13 @@
       <c r="E48" s="18"/>
       <c r="F48" s="18"/>
       <c r="G48" s="16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="16" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C49" s="18" t="s">
         <v>60</v>
@@ -1624,51 +1687,100 @@
       <c r="E49" s="18"/>
       <c r="F49" s="18"/>
       <c r="G49" s="16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="16" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C50" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D50" s="17"/>
+      <c r="D50" s="17" t="s">
+        <v>95</v>
+      </c>
       <c r="E50" s="18"/>
       <c r="F50" s="18"/>
       <c r="G50" s="16" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="16" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D51" s="18"/>
+        <v>60</v>
+      </c>
+      <c r="D51" s="17" t="s">
+        <v>96</v>
+      </c>
       <c r="E51" s="18"/>
       <c r="F51" s="18"/>
-      <c r="G51" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G51" s="16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="16" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D52" s="18"/>
+        <v>60</v>
+      </c>
+      <c r="D52" s="17"/>
       <c r="E52" s="18"/>
       <c r="F52" s="18"/>
-      <c r="G52" s="18" t="s">
+      <c r="G52" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+      <c r="B53" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D53" s="17"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+      <c r="B54" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+      <c r="B55" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C55" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D55" s="18"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="18" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Denied file uplod for object with DELETE and DELETED status.
Former-commit-id: c5e9c05821d2390c9640e8b021b783301e1ba448
</commit_message>
<xml_diff>
--- a/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-access-control-rules.xlsx
+++ b/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-access-control-rules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sasko.tanaskoski\.arkcase\acm\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\ArkCase\ACM3\acm-services\acm-service-data-access-control\src\main\resources\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -327,12 +327,6 @@
     <t>Task – Only participants can version files</t>
   </si>
   <si>
-    <t>status != 'CLOSED'</t>
-  </si>
-  <si>
-    <t>status == 'CLOSED'</t>
-  </si>
-  <si>
     <t>deny uploadOrReplaceFile to assignee, co-owner, supervisor, owning group, approver, collaborator</t>
   </si>
   <si>
@@ -346,6 +340,12 @@
   </si>
   <si>
     <t>deny uploadOrReplaceFile to assignee, co-owner, supervisor, owning group, approver, collaborator, reader</t>
+  </si>
+  <si>
+    <t>status != 'CLOSED' &amp;&amp; status != 'DELETE' &amp;&amp; status != 'DELETED'</t>
+  </si>
+  <si>
+    <t>status == 'CLOSED' || status == 'DELETE' || status == 'DELETED'</t>
   </si>
 </sst>
 </file>
@@ -579,7 +579,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -612,6 +612,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -999,8 +1002,8 @@
   </sheetPr>
   <dimension ref="A2:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1320,8 +1323,8 @@
       <c r="C26" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="17" t="s">
-        <v>95</v>
+      <c r="D26" s="20" t="s">
+        <v>100</v>
       </c>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
@@ -1332,18 +1335,18 @@
     <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C27" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="17" t="s">
-        <v>96</v>
+      <c r="D27" s="20" t="s">
+        <v>101</v>
       </c>
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
       <c r="G27" s="16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1559,8 +1562,8 @@
       <c r="C41" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D41" s="17" t="s">
-        <v>95</v>
+      <c r="D41" s="20" t="s">
+        <v>100</v>
       </c>
       <c r="E41" s="18"/>
       <c r="F41" s="18"/>
@@ -1571,18 +1574,18 @@
     <row r="42" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C42" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D42" s="17" t="s">
-        <v>96</v>
+      <c r="D42" s="20" t="s">
+        <v>101</v>
       </c>
       <c r="E42" s="18"/>
       <c r="F42" s="18"/>
       <c r="G42" s="16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1698,8 +1701,8 @@
       <c r="C50" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D50" s="17" t="s">
-        <v>95</v>
+      <c r="D50" s="20" t="s">
+        <v>100</v>
       </c>
       <c r="E50" s="18"/>
       <c r="F50" s="18"/>
@@ -1710,18 +1713,18 @@
     <row r="51" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C51" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D51" s="17" t="s">
-        <v>96</v>
+      <c r="D51" s="20" t="s">
+        <v>101</v>
       </c>
       <c r="E51" s="18"/>
       <c r="F51" s="18"/>
       <c r="G51" s="16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1786,7 +1789,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added * to participant list in drools rules. Refresh tree when upload denied.
Former-commit-id: 289af587f85eeefdcde402a7f614051142f3c10a
</commit_message>
<xml_diff>
--- a/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-access-control-rules.xlsx
+++ b/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-access-control-rules.xlsx
@@ -327,9 +327,6 @@
     <t>Task – Only participants can version files</t>
   </si>
   <si>
-    <t>deny uploadOrReplaceFile to assignee, co-owner, supervisor, owning group, approver, collaborator</t>
-  </si>
-  <si>
     <t>Case File – Participants cannot version files</t>
   </si>
   <si>
@@ -339,13 +336,16 @@
     <t>Complaint – Participants cannot upload or replace files</t>
   </si>
   <si>
-    <t>deny uploadOrReplaceFile to assignee, co-owner, supervisor, owning group, approver, collaborator, reader</t>
-  </si>
-  <si>
     <t>status != 'CLOSED' &amp;&amp; status != 'DELETE' &amp;&amp; status != 'DELETED'</t>
   </si>
   <si>
     <t>status == 'CLOSED' || status == 'DELETE' || status == 'DELETED'</t>
+  </si>
+  <si>
+    <t>deny uploadOrReplaceFile to assignee, co-owner, supervisor, owning group, approver, collaborator, reader, *</t>
+  </si>
+  <si>
+    <t>deny uploadOrReplaceFile to assignee, co-owner, supervisor, owning group, approver, collaborator, *</t>
   </si>
 </sst>
 </file>
@@ -1003,7 +1003,7 @@
   <dimension ref="A2:G55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1324,7 +1324,7 @@
         <v>31</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
@@ -1335,18 +1335,18 @@
     <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C27" s="18" t="s">
         <v>31</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
       <c r="G27" s="16" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1563,7 +1563,7 @@
         <v>45</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E41" s="18"/>
       <c r="F41" s="18"/>
@@ -1571,21 +1571,21 @@
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C42" s="18" t="s">
         <v>45</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E42" s="18"/>
       <c r="F42" s="18"/>
       <c r="G42" s="16" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1702,7 +1702,7 @@
         <v>60</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E50" s="18"/>
       <c r="F50" s="18"/>
@@ -1710,21 +1710,21 @@
         <v>76</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C51" s="18" t="s">
         <v>60</v>
       </c>
       <c r="D51" s="20" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E51" s="18"/>
       <c r="F51" s="18"/>
       <c r="G51" s="16" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Introduced addTag privilege to drools. Added privilege checking when adding tag.
Former-commit-id: a4d52d82ad709b5a7eed4144c6d4407c9d56d6a0
</commit_message>
<xml_diff>
--- a/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-access-control-rules.xlsx
+++ b/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-access-control-rules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="104">
   <si>
     <t>RuleSet</t>
   </si>
@@ -346,6 +346,12 @@
   </si>
   <si>
     <t>deny uploadOrReplaceFile to assignee, co-owner, supervisor, owning group, approver, collaborator, *</t>
+  </si>
+  <si>
+    <t>Task – Only participants can add tags</t>
+  </si>
+  <si>
+    <t>grant addTag to assignee, co-owner, supervisor, owning group, approver, collaborator, reader</t>
   </si>
 </sst>
 </file>
@@ -1000,10 +1006,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A2:G55"/>
+  <dimension ref="A2:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1757,25 +1763,25 @@
         <v>91</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="16" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="C54" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D54" s="18"/>
+        <v>60</v>
+      </c>
+      <c r="D54" s="17"/>
       <c r="E54" s="18"/>
       <c r="F54" s="18"/>
-      <c r="G54" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G54" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C55" s="18" t="s">
         <v>67</v>
@@ -1784,6 +1790,21 @@
       <c r="E55" s="18"/>
       <c r="F55" s="18"/>
       <c r="G55" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+      <c r="B56" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Do not authorize addTag for FILE object type.
Former-commit-id: e7cce2f82f48943cea3380561e3fe4e2676034b8
</commit_message>
<xml_diff>
--- a/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-access-control-rules.xlsx
+++ b/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-access-control-rules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\ArkCase\ACM3\acm-services\acm-service-data-access-control\src\main\resources\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sasko.tanaskoski\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="107">
   <si>
     <t>RuleSet</t>
   </si>
@@ -352,6 +352,15 @@
   </si>
   <si>
     <t>grant addTag to assignee, co-owner, supervisor, owning group, approver, collaborator, reader</t>
+  </si>
+  <si>
+    <t>Complaint – Anybody can add tag</t>
+  </si>
+  <si>
+    <t>grant addTag to *</t>
+  </si>
+  <si>
+    <t>Case File – anyone can add tag</t>
   </si>
 </sst>
 </file>
@@ -1006,10 +1015,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A2:G56"/>
+  <dimension ref="A2:G58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1388,86 +1397,86 @@
     <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>45</v>
+        <v>104</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>31</v>
       </c>
       <c r="D30" s="17"/>
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
-      <c r="G30" s="18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G30" s="16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C31" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D31" s="17" t="s">
-        <v>34</v>
-      </c>
+      <c r="D31" s="17"/>
       <c r="E31" s="18"/>
       <c r="F31" s="18"/>
-      <c r="G31" s="16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G31" s="18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C32" s="17" t="s">
         <v>45</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E32" s="18"/>
       <c r="F32" s="18"/>
-      <c r="G32" s="18" t="s">
-        <v>35</v>
+      <c r="G32" s="16" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="18"/>
+      <c r="D33" s="17" t="s">
+        <v>37</v>
+      </c>
       <c r="E33" s="18"/>
       <c r="F33" s="18"/>
       <c r="G33" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C34" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D34" s="17"/>
+      <c r="D34" s="18"/>
       <c r="E34" s="18"/>
       <c r="F34" s="18"/>
-      <c r="G34" s="16" t="s">
-        <v>41</v>
+      <c r="G34" s="18" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C35" s="18" t="s">
         <v>45</v>
@@ -1476,50 +1485,48 @@
       <c r="E35" s="18"/>
       <c r="F35" s="18"/>
       <c r="G35" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C36" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D36" s="17" t="s">
-        <v>53</v>
-      </c>
+      <c r="D36" s="17"/>
       <c r="E36" s="18"/>
       <c r="F36" s="18"/>
       <c r="G36" s="16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>56</v>
+        <v>45</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>53</v>
       </c>
       <c r="E37" s="18"/>
       <c r="F37" s="18"/>
-      <c r="G37" s="18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G37" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D38" s="18" t="s">
         <v>56</v>
@@ -1530,25 +1537,27 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="16" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="C39" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D39" s="17"/>
+      <c r="D39" s="18" t="s">
+        <v>56</v>
+      </c>
       <c r="E39" s="18"/>
       <c r="F39" s="18"/>
-      <c r="G39" s="16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G39" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="16" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="C40" s="18" t="s">
         <v>45</v>
@@ -1557,62 +1566,62 @@
       <c r="E40" s="18"/>
       <c r="F40" s="18"/>
       <c r="G40" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="16" t="s">
-        <v>85</v>
+        <v>51</v>
       </c>
       <c r="C41" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D41" s="20" t="s">
-        <v>98</v>
-      </c>
+      <c r="D41" s="17"/>
       <c r="E41" s="18"/>
       <c r="F41" s="18"/>
       <c r="G41" s="16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="16" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C42" s="18" t="s">
         <v>45</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E42" s="18"/>
       <c r="F42" s="18"/>
       <c r="G42" s="16" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="16" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="C43" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D43" s="17"/>
+      <c r="D43" s="20" t="s">
+        <v>99</v>
+      </c>
       <c r="E43" s="18"/>
       <c r="F43" s="18"/>
       <c r="G43" s="16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C44" s="18" t="s">
         <v>45</v>
@@ -1621,58 +1630,58 @@
       <c r="E44" s="18"/>
       <c r="F44" s="18"/>
       <c r="G44" s="16" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="16" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D45" s="18"/>
+        <v>45</v>
+      </c>
+      <c r="D45" s="17"/>
       <c r="E45" s="18"/>
       <c r="F45" s="18"/>
-      <c r="G45" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G45" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="16" t="s">
-        <v>61</v>
+        <v>106</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="D46" s="17"/>
       <c r="E46" s="18"/>
       <c r="F46" s="18"/>
       <c r="G46" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C47" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D47" s="17"/>
+      <c r="D47" s="18"/>
       <c r="E47" s="18"/>
       <c r="F47" s="18"/>
-      <c r="G47" s="16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G47" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C48" s="18" t="s">
         <v>60</v>
@@ -1681,13 +1690,13 @@
       <c r="E48" s="18"/>
       <c r="F48" s="18"/>
       <c r="G48" s="16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="16" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="C49" s="18" t="s">
         <v>60</v>
@@ -1696,77 +1705,77 @@
       <c r="E49" s="18"/>
       <c r="F49" s="18"/>
       <c r="G49" s="16" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="16" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="C50" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D50" s="20" t="s">
-        <v>98</v>
-      </c>
+      <c r="D50" s="17"/>
       <c r="E50" s="18"/>
       <c r="F50" s="18"/>
       <c r="G50" s="16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="16" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C51" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D51" s="20" t="s">
-        <v>99</v>
-      </c>
+      <c r="D51" s="17"/>
       <c r="E51" s="18"/>
       <c r="F51" s="18"/>
       <c r="G51" s="16" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="16" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C52" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D52" s="17"/>
+      <c r="D52" s="20" t="s">
+        <v>98</v>
+      </c>
       <c r="E52" s="18"/>
       <c r="F52" s="18"/>
       <c r="G52" s="16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="16" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C53" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D53" s="17"/>
+      <c r="D53" s="20" t="s">
+        <v>99</v>
+      </c>
       <c r="E53" s="18"/>
       <c r="F53" s="18"/>
       <c r="G53" s="16" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="16" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C54" s="18" t="s">
         <v>60</v>
@@ -1775,36 +1784,66 @@
       <c r="E54" s="18"/>
       <c r="F54" s="18"/>
       <c r="G54" s="16" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="16" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="C55" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D55" s="18"/>
+        <v>60</v>
+      </c>
+      <c r="D55" s="17"/>
       <c r="E55" s="18"/>
       <c r="F55" s="18"/>
-      <c r="G55" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G55" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="16" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D56" s="18"/>
+        <v>60</v>
+      </c>
+      <c r="D56" s="17"/>
       <c r="E56" s="18"/>
       <c r="F56" s="18"/>
-      <c r="G56" s="18" t="s">
+      <c r="G56" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="1"/>
+      <c r="B57" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="1"/>
+      <c r="B58" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C58" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D58" s="18"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="18"/>
+      <c r="G58" s="18" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AFDP-9099 Update data access control rules xslx, fix broken case file, consultation and data access tests and add consultation data access rules test
</commit_message>
<xml_diff>
--- a/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-access-control-rules.xlsx
+++ b/acm-services/acm-service-data-access-control/src/main/resources/rules/drools-access-control-rules.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sasko.tanaskoski\.arkcase\acm\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleksandar.acevski\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D5AF28-FEB8-4C96-99C1-7B375A6A672B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="169"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +21,17 @@
     <definedName name="ObjectTypes">Sheet2!$A$2:$A$51</definedName>
     <definedName name="ParticipantTypes">Sheet2!$B$2:$B$51</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="163">
   <si>
     <t>RuleSet</t>
   </si>
@@ -165,13 +171,37 @@
     <t>Complaint – Only participants can add files</t>
   </si>
   <si>
-    <t>grant add file to assignee, co-owner, supervisor, owning group, approver, collaborator</t>
-  </si>
-  <si>
     <t>Complaint – Only participants can save</t>
   </si>
   <si>
-    <t>grant save to assignee, co-owner, supervisor, owning group, approver, collaborator</t>
+    <t>Complaint – Everyone can upload or replace files</t>
+  </si>
+  <si>
+    <t>status != 'CLOSED' &amp;&amp; status != 'DELETE' &amp;&amp; status != 'DELETED'</t>
+  </si>
+  <si>
+    <t>Complaint – Deny upload or replace files on closed complaint</t>
+  </si>
+  <si>
+    <t>status == 'CLOSED' || status == 'DELETE' || status == 'DELETED'</t>
+  </si>
+  <si>
+    <t>Complaint – Anybody can add comments</t>
+  </si>
+  <si>
+    <t>grant addComment to *</t>
+  </si>
+  <si>
+    <t>Complaint – Anybody can subscribe</t>
+  </si>
+  <si>
+    <t>grant subscribe to *</t>
+  </si>
+  <si>
+    <t>Complaint – Anybody can add tag</t>
+  </si>
+  <si>
+    <t>grant addTag to *</t>
   </si>
   <si>
     <t>Case File – Assignee Read Access</t>
@@ -183,9 +213,6 @@
     <t>Case File – Grant Participants Access to Drafts</t>
   </si>
   <si>
-    <t>grant read to assignee, co-owner, supervisor, owning group, approver, collaborator, follower, reader</t>
-  </si>
-  <si>
     <t>Case File – Grant Access to non-Drafts</t>
   </si>
   <si>
@@ -204,9 +231,6 @@
     <t>status == 'DELETED'</t>
   </si>
   <si>
-    <t>mandatory deny read to assignee, co-owner, supervisor, owning group, approver, collaborator, *</t>
-  </si>
-  <si>
     <t>Complaint – Restricted Flag</t>
   </si>
   <si>
@@ -219,6 +243,24 @@
     <t>Case File – Restricted Flag</t>
   </si>
   <si>
+    <t>Case File – Only participants can view details page</t>
+  </si>
+  <si>
+    <t>Case File – Everyone can upload or replace files</t>
+  </si>
+  <si>
+    <t>Case File –  Deny upload or replace files on closed case file</t>
+  </si>
+  <si>
+    <t>Case File – Only participants can add comments</t>
+  </si>
+  <si>
+    <t>Case File – anyone can subscribe</t>
+  </si>
+  <si>
+    <t>Case File – anyone can add tag</t>
+  </si>
+  <si>
     <t>Task – default read access</t>
   </si>
   <si>
@@ -237,16 +279,124 @@
     <t>grant complete to assignee</t>
   </si>
   <si>
+    <t>Task – Only assignee and supervisor can delete</t>
+  </si>
+  <si>
     <t>grant delete to assignee, supervisor</t>
   </si>
   <si>
-    <t>Folder – default public access</t>
+    <t>Task – Everyone can upload or replace files</t>
+  </si>
+  <si>
+    <t>Task –  Deny upload or replace files on closed complaint</t>
+  </si>
+  <si>
+    <t>Task – Only participants can add comments</t>
+  </si>
+  <si>
+    <t>Task – anybody can subscribe</t>
+  </si>
+  <si>
+    <t>grant subscribe to subscribe</t>
+  </si>
+  <si>
+    <t>Task – Only participants can add tags</t>
+  </si>
+  <si>
+    <t>Folder - default list folder</t>
   </si>
   <si>
     <t>FOLDER</t>
   </si>
   <si>
-    <t>Folder –deny no access</t>
+    <t>grant read to group-write, group-read, write, read, *</t>
+  </si>
+  <si>
+    <t>Folder - write to folder</t>
+  </si>
+  <si>
+    <t>grant write to group-write, write</t>
+  </si>
+  <si>
+    <t>Folder – deny no access</t>
+  </si>
+  <si>
+    <t>mandatory deny read to no-access, group-no-access</t>
+  </si>
+  <si>
+    <t>Folder – Restricted Flag</t>
+  </si>
+  <si>
+    <t>File - default read file</t>
+  </si>
+  <si>
+    <t>FILE</t>
+  </si>
+  <si>
+    <t>File - write</t>
+  </si>
+  <si>
+    <t>File – deny no access</t>
+  </si>
+  <si>
+    <t>File – Restricted Flag</t>
+  </si>
+  <si>
+    <t>Document Repository -default read access</t>
+  </si>
+  <si>
+    <t>DOC_REPO</t>
+  </si>
+  <si>
+    <t>DocumentRepository – Anybody can add comments</t>
+  </si>
+  <si>
+    <t>DocumentRepository – Lockout No Access Users</t>
+  </si>
+  <si>
+    <t>DocumentRepository – Anybody can add tag</t>
+  </si>
+  <si>
+    <t>DocumentRepository – Anybody can subscribe</t>
+  </si>
+  <si>
+    <t>DocumentRepository – Restricted Flag</t>
+  </si>
+  <si>
+    <t>DocumentRepository – Everyone can upload or replace files</t>
+  </si>
+  <si>
+    <t>DocumentRepository – Only participants can save</t>
+  </si>
+  <si>
+    <t>Organization – Lockout No Access Users</t>
+  </si>
+  <si>
+    <t>ORGANIZATION</t>
+  </si>
+  <si>
+    <t>Organization – default read access</t>
+  </si>
+  <si>
+    <t>Organization – Only participants can save</t>
+  </si>
+  <si>
+    <t>Organization – Restricted Flag</t>
+  </si>
+  <si>
+    <t>Person – Lockout No Access Users</t>
+  </si>
+  <si>
+    <t>PERSON</t>
+  </si>
+  <si>
+    <t>Person – default read access</t>
+  </si>
+  <si>
+    <t>Person – Only participants can save</t>
+  </si>
+  <si>
+    <t>Person – Restricted Flag</t>
   </si>
   <si>
     <t>Object Types</t>
@@ -261,112 +411,136 @@
     <t>Owner's Supervisor</t>
   </si>
   <si>
-    <t>FILE</t>
-  </si>
-  <si>
     <t>PARTICIPANT</t>
   </si>
   <si>
     <t>ACCESS CONTROL LIST</t>
   </si>
   <si>
-    <t>grant uploadOrReplaceFile to assignee, co-owner, supervisor, owning group, approver, collaborator</t>
-  </si>
-  <si>
-    <t>Complaint – Only participants can upload or replace files</t>
-  </si>
-  <si>
-    <t>Complaint – Anybody can add comments</t>
-  </si>
-  <si>
-    <t>Complaint – Anybody can subscribe</t>
-  </si>
-  <si>
-    <t>grant addComment to *</t>
-  </si>
-  <si>
-    <t>grant subscribe to *</t>
-  </si>
-  <si>
-    <t>grant viewCaseDetailsPage to assignee, co-owner, supervisor, owning group, approver, collaborator, reader</t>
-  </si>
-  <si>
-    <t>grant saveCase to assignee, co-owner, supervisor, owning group, approver, collaborator</t>
-  </si>
-  <si>
-    <t>Case File – Only participants can view details page</t>
-  </si>
-  <si>
-    <t>Case File – Only participants can version files</t>
-  </si>
-  <si>
-    <t>grant uploadOrReplaceFile to assignee, co-owner, supervisor, owning group, approver, collaborator, reader</t>
-  </si>
-  <si>
-    <t>grant addComment to assignee, co-owner, supervisor, owning group, approver, collaborator, reader</t>
-  </si>
-  <si>
-    <t>Case File – Only participants can add comments</t>
-  </si>
-  <si>
-    <t>Case File – anyone can subscribe</t>
-  </si>
-  <si>
-    <t>Task – Only assignee and supervisor can delete</t>
-  </si>
-  <si>
-    <t>grant subscribe to subscribe</t>
-  </si>
-  <si>
-    <t>Task – anybody can subscribe</t>
-  </si>
-  <si>
-    <t>Task – Only participants can add comments</t>
-  </si>
-  <si>
-    <t>Task – Only participants can version files</t>
-  </si>
-  <si>
-    <t>Case File – Participants cannot version files</t>
-  </si>
-  <si>
-    <t>Task – Participants cannot version files</t>
-  </si>
-  <si>
-    <t>Complaint – Participants cannot upload or replace files</t>
-  </si>
-  <si>
-    <t>status != 'CLOSED' &amp;&amp; status != 'DELETE' &amp;&amp; status != 'DELETED'</t>
-  </si>
-  <si>
-    <t>status == 'CLOSED' || status == 'DELETE' || status == 'DELETED'</t>
-  </si>
-  <si>
-    <t>deny uploadOrReplaceFile to assignee, co-owner, supervisor, owning group, approver, collaborator, reader, *</t>
-  </si>
-  <si>
-    <t>deny uploadOrReplaceFile to assignee, co-owner, supervisor, owning group, approver, collaborator, *</t>
-  </si>
-  <si>
-    <t>Task – Only participants can add tags</t>
-  </si>
-  <si>
-    <t>grant addTag to assignee, co-owner, supervisor, owning group, approver, collaborator, reader</t>
-  </si>
-  <si>
-    <t>Complaint – Anybody can add tag</t>
-  </si>
-  <si>
-    <t>grant addTag to *</t>
-  </si>
-  <si>
-    <t>Case File – anyone can add tag</t>
+    <t>Costsheet – Only participants can add files</t>
+  </si>
+  <si>
+    <t>COSTSHEET</t>
+  </si>
+  <si>
+    <t>Costsheet – default read access</t>
+  </si>
+  <si>
+    <t>Costsheet – Only participants can save</t>
+  </si>
+  <si>
+    <t>Costsheet –  Only participants can upload or replace files</t>
+  </si>
+  <si>
+    <t>BUSINESS_PROCESS</t>
+  </si>
+  <si>
+    <t>BusinessProcess – Grant Access</t>
+  </si>
+  <si>
+    <t>grant add file to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator</t>
+  </si>
+  <si>
+    <t>grant save to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator</t>
+  </si>
+  <si>
+    <t>grant uploadOrReplaceFile to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator, reader, follower,  *</t>
+  </si>
+  <si>
+    <t>deny uploadOrReplaceFile to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator, reader, follower, *</t>
+  </si>
+  <si>
+    <t>grant read to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator, follower, reader</t>
+  </si>
+  <si>
+    <t>mandatory deny read to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator, *</t>
+  </si>
+  <si>
+    <t>grant viewCaseDetailsPage to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator, reader</t>
+  </si>
+  <si>
+    <t>grant saveCase to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator</t>
+  </si>
+  <si>
+    <t>grant uploadOrReplaceFile to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator, reader, follower, *</t>
+  </si>
+  <si>
+    <t>grant addComment to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator, reader</t>
+  </si>
+  <si>
+    <t>grant addTag to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator, reader</t>
+  </si>
+  <si>
+    <t>grant read to owner, owning group, collaborator group, collaborator, reader, *</t>
+  </si>
+  <si>
+    <t>grant add file to owner, owning group, collaborator group, collaborator, *</t>
+  </si>
+  <si>
+    <t>grant uploadOrReplaceFile to  owner, owning group, collaborator group, collaborator, *</t>
+  </si>
+  <si>
+    <t>grant save to owner, owning group, collaborator group, collaborator</t>
+  </si>
+  <si>
+    <t>grant add file to assignee, owner, co-owner, supervisor, owning group, collaborator group, approver, collaborator</t>
+  </si>
+  <si>
+    <t>grant save to assignee, owner, co-owner, supervisor, owning group, collaborator group, approver, collaborator</t>
+  </si>
+  <si>
+    <t>grant uploadOrReplaceFile to assignee, owner, co-owner, supervisor, owning group, collaborator group, approver, collaborator</t>
+  </si>
+  <si>
+    <t>Consultation – Assignee Read Access</t>
+  </si>
+  <si>
+    <t>Consultation – Grant Participants Access to Drafts</t>
+  </si>
+  <si>
+    <t>Consultation – Grant Access to non-Drafts</t>
+  </si>
+  <si>
+    <t>Consultation – Lockout No Access Users</t>
+  </si>
+  <si>
+    <t>Consultation – Only participants can add files</t>
+  </si>
+  <si>
+    <t>Consultation – Only participants can save</t>
+  </si>
+  <si>
+    <t>Consultation – Deleted Cases</t>
+  </si>
+  <si>
+    <t>Consultation – Restricted Flag</t>
+  </si>
+  <si>
+    <t>Consultation – Only participants can view details page</t>
+  </si>
+  <si>
+    <t>Consultation – Everyone can upload or replace files</t>
+  </si>
+  <si>
+    <t>Consultation –  Deny upload or replace files on closed Consultation</t>
+  </si>
+  <si>
+    <t>Consultation – Only participants can add comments</t>
+  </si>
+  <si>
+    <t>Consultation – anyone can subscribe</t>
+  </si>
+  <si>
+    <t>Consultation – anyone can add tag</t>
+  </si>
+  <si>
+    <t>CONSULTATION</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
@@ -732,7 +906,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -744,7 +918,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -1011,29 +1185,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A2:G58"/>
+  <dimension ref="A2:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.5703125"/>
-    <col min="2" max="2" width="24.28515625"/>
-    <col min="3" max="3" width="49.85546875"/>
-    <col min="4" max="4" width="36.140625"/>
-    <col min="5" max="5" width="43.85546875"/>
-    <col min="6" max="6" width="30.5703125"/>
-    <col min="7" max="7" width="35.5703125"/>
-    <col min="8" max="1025" width="8.7109375"/>
+    <col min="1" max="1" width="21.59765625" customWidth="1"/>
+    <col min="2" max="2" width="24.265625" customWidth="1"/>
+    <col min="3" max="3" width="49.86328125" customWidth="1"/>
+    <col min="4" max="4" width="36.1328125" customWidth="1"/>
+    <col min="5" max="5" width="43.86328125" customWidth="1"/>
+    <col min="6" max="6" width="30.59765625" customWidth="1"/>
+    <col min="7" max="7" width="35.59765625" customWidth="1"/>
+    <col min="8" max="1025" width="8.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -1043,7 +1217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -1053,7 +1227,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -1063,7 +1237,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -1073,7 +1247,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -1083,7 +1257,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -1093,7 +1267,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -1103,7 +1277,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -1113,7 +1287,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -1123,7 +1297,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
@@ -1133,7 +1307,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="360" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="327.75" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="4" t="s">
@@ -1143,7 +1317,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="7" t="s">
@@ -1153,7 +1327,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
@@ -1164,7 +1338,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="4" t="s">
@@ -1183,7 +1357,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="4" t="s">
@@ -1194,7 +1368,7 @@
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="10" t="s">
@@ -1213,7 +1387,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A19" s="11" t="s">
         <v>23</v>
       </c>
@@ -1236,7 +1410,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
       <c r="B20" s="16" t="s">
         <v>30</v>
@@ -1251,7 +1425,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A21" s="1"/>
       <c r="B21" s="16" t="s">
         <v>33</v>
@@ -1268,7 +1442,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A22" s="1"/>
       <c r="B22" s="16" t="s">
         <v>36</v>
@@ -1285,7 +1459,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A23" s="1"/>
       <c r="B23" s="16" t="s">
         <v>38</v>
@@ -1300,7 +1474,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A24" s="1"/>
       <c r="B24" s="16" t="s">
         <v>40</v>
@@ -1312,13 +1486,13 @@
       <c r="E24" s="18"/>
       <c r="F24" s="18"/>
       <c r="G24" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A25" s="1"/>
       <c r="B25" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C25" s="18" t="s">
         <v>31</v>
@@ -1327,47 +1501,47 @@
       <c r="E25" s="18"/>
       <c r="F25" s="18"/>
       <c r="G25" s="16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A26" s="1"/>
       <c r="B26" s="16" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="C26" s="18" t="s">
         <v>31</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>98</v>
+        <v>43</v>
       </c>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
       <c r="G26" s="16" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A27" s="1"/>
       <c r="B27" s="16" t="s">
-        <v>97</v>
+        <v>44</v>
       </c>
       <c r="C27" s="18" t="s">
         <v>31</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>99</v>
+        <v>45</v>
       </c>
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
       <c r="G27" s="16" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A28" s="1"/>
       <c r="B28" s="16" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="C28" s="18" t="s">
         <v>31</v>
@@ -1376,13 +1550,13 @@
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
       <c r="G28" s="16" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A29" s="1"/>
       <c r="B29" s="16" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
       <c r="C29" s="18" t="s">
         <v>31</v>
@@ -1391,13 +1565,13 @@
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
       <c r="G29" s="16" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A30" s="1"/>
       <c r="B30" s="16" t="s">
-        <v>104</v>
+        <v>50</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>31</v>
@@ -1406,455 +1580,1105 @@
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
       <c r="G30" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="1"/>
       <c r="B31" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D31" s="17"/>
+        <v>61</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>62</v>
+      </c>
       <c r="E31" s="18"/>
       <c r="F31" s="18"/>
       <c r="G31" s="18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A32" s="1"/>
       <c r="B32" s="16" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D32" s="17" t="s">
-        <v>34</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="D32" s="17"/>
       <c r="E32" s="18"/>
       <c r="F32" s="18"/>
-      <c r="G32" s="16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G32" s="18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A33" s="1"/>
       <c r="B33" s="16" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E33" s="18"/>
       <c r="F33" s="18"/>
-      <c r="G33" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G33" s="16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A34" s="1"/>
       <c r="B34" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="D34" s="18"/>
+        <v>55</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>37</v>
+      </c>
       <c r="E34" s="18"/>
       <c r="F34" s="18"/>
       <c r="G34" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A35" s="1"/>
       <c r="B35" s="16" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="D35" s="17"/>
+        <v>53</v>
+      </c>
+      <c r="D35" s="18"/>
       <c r="E35" s="18"/>
       <c r="F35" s="18"/>
-      <c r="G35" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G35" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A36" s="1"/>
       <c r="B36" s="16" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D36" s="17"/>
       <c r="E36" s="18"/>
       <c r="F36" s="18"/>
       <c r="G36" s="16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A37" s="1"/>
       <c r="B37" s="16" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="D37" s="17" t="s">
         <v>53</v>
       </c>
+      <c r="D37" s="17"/>
       <c r="E37" s="18"/>
       <c r="F37" s="18"/>
       <c r="G37" s="16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A38" s="1"/>
       <c r="B38" s="16" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D38" s="18" t="s">
-        <v>56</v>
+        <v>53</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>60</v>
       </c>
       <c r="E38" s="18"/>
       <c r="F38" s="18"/>
-      <c r="G38" s="18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G38" s="16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="1"/>
       <c r="B39" s="16" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="E39" s="18"/>
       <c r="F39" s="18"/>
       <c r="G39" s="18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A40" s="1"/>
       <c r="B40" s="16" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D40" s="17"/>
       <c r="E40" s="18"/>
       <c r="F40" s="18"/>
       <c r="G40" s="16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A41" s="1"/>
       <c r="B41" s="16" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D41" s="17"/>
       <c r="E41" s="18"/>
       <c r="F41" s="18"/>
       <c r="G41" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A42" s="1"/>
       <c r="B42" s="16" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>98</v>
+        <v>43</v>
       </c>
       <c r="E42" s="18"/>
       <c r="F42" s="18"/>
       <c r="G42" s="16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A43" s="1"/>
       <c r="B43" s="16" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="C43" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D43" s="20" t="s">
         <v>45</v>
-      </c>
-      <c r="D43" s="20" t="s">
-        <v>99</v>
       </c>
       <c r="E43" s="18"/>
       <c r="F43" s="18"/>
       <c r="G43" s="16" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A44" s="1"/>
       <c r="B44" s="16" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D44" s="17"/>
       <c r="E44" s="18"/>
       <c r="F44" s="18"/>
       <c r="G44" s="16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A45" s="1"/>
       <c r="B45" s="16" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D45" s="17"/>
       <c r="E45" s="18"/>
       <c r="F45" s="18"/>
       <c r="G45" s="16" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A46" s="1"/>
       <c r="B46" s="16" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D46" s="17"/>
       <c r="E46" s="18"/>
       <c r="F46" s="18"/>
       <c r="G46" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A47" s="1"/>
       <c r="B47" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C47" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D47" s="18"/>
+        <v>148</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="D47" s="17"/>
       <c r="E47" s="18"/>
       <c r="F47" s="18"/>
       <c r="G47" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A48" s="1"/>
       <c r="B48" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="C48" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D48" s="17"/>
+        <v>149</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="D48" s="17" t="s">
+        <v>34</v>
+      </c>
       <c r="E48" s="18"/>
       <c r="F48" s="18"/>
       <c r="G48" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A49" s="1"/>
       <c r="B49" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C49" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D49" s="17"/>
+        <v>150</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="D49" s="17" t="s">
+        <v>37</v>
+      </c>
       <c r="E49" s="18"/>
       <c r="F49" s="18"/>
-      <c r="G49" s="16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G49" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A50" s="1"/>
       <c r="B50" s="16" t="s">
-        <v>63</v>
+        <v>151</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D50" s="17"/>
+        <v>162</v>
+      </c>
+      <c r="D50" s="18"/>
       <c r="E50" s="18"/>
       <c r="F50" s="18"/>
-      <c r="G50" s="16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G50" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A51" s="1"/>
       <c r="B51" s="16" t="s">
-        <v>90</v>
+        <v>152</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>60</v>
+        <v>162</v>
       </c>
       <c r="D51" s="17"/>
       <c r="E51" s="18"/>
       <c r="F51" s="18"/>
       <c r="G51" s="16" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A52" s="1"/>
       <c r="B52" s="16" t="s">
-        <v>94</v>
+        <v>153</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D52" s="20" t="s">
-        <v>98</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="D52" s="17"/>
       <c r="E52" s="18"/>
       <c r="F52" s="18"/>
       <c r="G52" s="16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A53" s="1"/>
       <c r="B53" s="16" t="s">
-        <v>96</v>
+        <v>154</v>
       </c>
       <c r="C53" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="D53" s="17" t="s">
         <v>60</v>
-      </c>
-      <c r="D53" s="20" t="s">
-        <v>99</v>
       </c>
       <c r="E53" s="18"/>
       <c r="F53" s="18"/>
       <c r="G53" s="16" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="1"/>
       <c r="B54" s="16" t="s">
-        <v>93</v>
+        <v>155</v>
       </c>
       <c r="C54" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D54" s="17"/>
+        <v>162</v>
+      </c>
+      <c r="D54" s="18" t="s">
+        <v>62</v>
+      </c>
       <c r="E54" s="18"/>
       <c r="F54" s="18"/>
-      <c r="G54" s="16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G54" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A55" s="1"/>
       <c r="B55" s="16" t="s">
-        <v>92</v>
+        <v>156</v>
       </c>
       <c r="C55" s="18" t="s">
-        <v>60</v>
+        <v>162</v>
       </c>
       <c r="D55" s="17"/>
       <c r="E55" s="18"/>
       <c r="F55" s="18"/>
       <c r="G55" s="16" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A56" s="1"/>
       <c r="B56" s="16" t="s">
-        <v>102</v>
+        <v>153</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>60</v>
+        <v>162</v>
       </c>
       <c r="D56" s="17"/>
       <c r="E56" s="18"/>
       <c r="F56" s="18"/>
       <c r="G56" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A57" s="1"/>
       <c r="B57" s="16" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C57" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D57" s="18"/>
+        <v>162</v>
+      </c>
+      <c r="D57" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="E57" s="18"/>
       <c r="F57" s="18"/>
-      <c r="G57" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G57" s="16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A58" s="1"/>
       <c r="B58" s="16" t="s">
-        <v>68</v>
+        <v>158</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D58" s="18"/>
+        <v>162</v>
+      </c>
+      <c r="D58" s="20" t="s">
+        <v>45</v>
+      </c>
       <c r="E58" s="18"/>
       <c r="F58" s="18"/>
-      <c r="G58" s="18" t="s">
+      <c r="G58" s="16" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A59" s="1"/>
+      <c r="B59" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="D59" s="17"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="18"/>
+      <c r="G59" s="16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A60" s="1"/>
+      <c r="B60" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="C60" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="D60" s="17"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18"/>
+      <c r="G60" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A61" s="1"/>
+      <c r="B61" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="C61" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="D61" s="17"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
+      <c r="G61" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A62" s="1"/>
+      <c r="B62" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C62" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D62" s="18"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="18"/>
+      <c r="G62" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A63" s="1"/>
+      <c r="B63" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C63" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D63" s="17"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="18"/>
+      <c r="G63" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A64" s="1"/>
+      <c r="B64" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C64" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D64" s="17"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="18"/>
+      <c r="G64" s="16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A65" s="1"/>
+      <c r="B65" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C65" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D65" s="17"/>
+      <c r="E65" s="18"/>
+      <c r="F65" s="18"/>
+      <c r="G65" s="16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A66" s="1"/>
+      <c r="B66" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C66" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D66" s="17"/>
+      <c r="E66" s="18"/>
+      <c r="F66" s="18"/>
+      <c r="G66" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+      <c r="A67" s="1"/>
+      <c r="B67" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C67" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D67" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E67" s="18"/>
+      <c r="F67" s="18"/>
+      <c r="G67" s="16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+      <c r="A68" s="1"/>
+      <c r="B68" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C68" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D68" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="E68" s="18"/>
+      <c r="F68" s="18"/>
+      <c r="G68" s="16" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A69" s="1"/>
+      <c r="B69" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C69" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D69" s="17"/>
+      <c r="E69" s="18"/>
+      <c r="F69" s="18"/>
+      <c r="G69" s="16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A70" s="1"/>
+      <c r="B70" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C70" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D70" s="17"/>
+      <c r="E70" s="18"/>
+      <c r="F70" s="18"/>
+      <c r="G70" s="16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A71" s="1"/>
+      <c r="B71" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C71" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D71" s="17"/>
+      <c r="E71" s="18"/>
+      <c r="F71" s="18"/>
+      <c r="G71" s="16" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A72" s="1"/>
+      <c r="B72" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C72" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D72" s="18"/>
+      <c r="E72" s="18"/>
+      <c r="F72" s="18"/>
+      <c r="G72" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A73" s="1"/>
+      <c r="B73" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C73" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D73" s="18"/>
+      <c r="E73" s="18"/>
+      <c r="F73" s="18"/>
+      <c r="G73" s="16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A74" s="1"/>
+      <c r="B74" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C74" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D74" s="18"/>
+      <c r="E74" s="18"/>
+      <c r="F74" s="18"/>
+      <c r="G74" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A75" s="1"/>
+      <c r="B75" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C75" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D75" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E75" s="18"/>
+      <c r="F75" s="18"/>
+      <c r="G75" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A76" s="1"/>
+      <c r="B76" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C76" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D76" s="18"/>
+      <c r="E76" s="18"/>
+      <c r="F76" s="18"/>
+      <c r="G76" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A77" s="1"/>
+      <c r="B77" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C77" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D77" s="18"/>
+      <c r="E77" s="18"/>
+      <c r="F77" s="18"/>
+      <c r="G77" s="16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A78" s="1"/>
+      <c r="B78" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C78" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D78" s="18"/>
+      <c r="E78" s="18"/>
+      <c r="F78" s="18"/>
+      <c r="G78" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A79" s="1"/>
+      <c r="B79" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C79" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D79" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E79" s="18"/>
+      <c r="F79" s="18"/>
+      <c r="G79" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A80" s="1"/>
+      <c r="B80" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C80" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D80" s="18"/>
+      <c r="E80" s="18"/>
+      <c r="F80" s="18"/>
+      <c r="G80" s="16" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B81" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C81" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="D81" s="16"/>
+      <c r="E81" s="16"/>
+      <c r="F81" s="16"/>
+      <c r="G81" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B82" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C82" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="D82" s="16"/>
+      <c r="E82" s="16"/>
+      <c r="F82" s="16"/>
+      <c r="G82" s="16" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B83" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="C83" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="D83" s="16"/>
+      <c r="E83" s="16"/>
+      <c r="F83" s="16"/>
+      <c r="G83" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B84" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C84" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="D84" s="16"/>
+      <c r="E84" s="16"/>
+      <c r="F84" s="16"/>
+      <c r="G84" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B85" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C85" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D85" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E85" s="18"/>
+      <c r="F85" s="18"/>
+      <c r="G85" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B86" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="C86" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D86" s="17"/>
+      <c r="E86" s="18"/>
+      <c r="F86" s="18"/>
+      <c r="G86" s="16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="87" spans="2:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B87" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="C87" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D87" s="17"/>
+      <c r="E87" s="18"/>
+      <c r="F87" s="18"/>
+      <c r="G87" s="16" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B88" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C88" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D88" s="17"/>
+      <c r="E88" s="18"/>
+      <c r="F88" s="18"/>
+      <c r="G88" s="16" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B89" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C89" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="D89" s="17"/>
+      <c r="E89" s="18"/>
+      <c r="F89" s="18"/>
+      <c r="G89" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B90" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C90" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="D90" s="17"/>
+      <c r="E90" s="18"/>
+      <c r="F90" s="18"/>
+      <c r="G90" s="16" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B91" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C91" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="D91" s="17"/>
+      <c r="E91" s="18"/>
+      <c r="F91" s="18"/>
+      <c r="G91" s="16" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B92" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C92" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D92" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E92" s="18"/>
+      <c r="F92" s="18"/>
+      <c r="G92" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B93" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C93" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="D93" s="17"/>
+      <c r="E93" s="18"/>
+      <c r="F93" s="18"/>
+      <c r="G93" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B94" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="C94" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="D94" s="17"/>
+      <c r="E94" s="18"/>
+      <c r="F94" s="18"/>
+      <c r="G94" s="16" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="95" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B95" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C95" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="D95" s="17"/>
+      <c r="E95" s="18"/>
+      <c r="F95" s="18"/>
+      <c r="G95" s="16" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B96" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="C96" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="D96" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E96" s="18"/>
+      <c r="F96" s="18"/>
+      <c r="G96" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A97" s="1"/>
+      <c r="B97" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="C97" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="D97" s="18"/>
+      <c r="E97" s="18"/>
+      <c r="F97" s="18"/>
+      <c r="G97" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A98" s="1"/>
+      <c r="B98" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C98" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="D98" s="17"/>
+      <c r="E98" s="18"/>
+      <c r="F98" s="18"/>
+      <c r="G98" s="16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A99" s="1"/>
+      <c r="B99" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="C99" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="D99" s="17"/>
+      <c r="E99" s="18"/>
+      <c r="F99" s="18"/>
+      <c r="G99" s="16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+      <c r="A100" s="1"/>
+      <c r="B100" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="C100" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="D100" s="20"/>
+      <c r="E100" s="18"/>
+      <c r="F100" s="18"/>
+      <c r="G100" s="16" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B101" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="C101" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="D101" s="17"/>
+      <c r="E101" s="18"/>
+      <c r="F101" s="18"/>
+      <c r="G101" s="18" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
@@ -1864,60 +2688,60 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.7109375"/>
-    <col min="2" max="2" width="17.5703125"/>
-    <col min="3" max="1025" width="8.7109375"/>
+    <col min="1" max="1" width="18.73046875" customWidth="1"/>
+    <col min="2" max="2" width="17.59765625" customWidth="1"/>
+    <col min="3" max="1025" width="8.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>117</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
@@ -1925,12 +2749,12 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1025" width="8.7109375"/>
+    <col min="1" max="1025" width="8.73046875" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>